<commit_message>
plots and tft exps
</commit_message>
<xml_diff>
--- a/src/TFT_experiments.xlsx
+++ b/src/TFT_experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,125 +483,125 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>model_week_365_72</t>
+          <t>model_month_113_72</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10.83476448059082</v>
+        <v>1.618298530578613</v>
       </c>
       <c r="C2" t="n">
         <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4696487911301886</v>
+        <v>0.01</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1039155309883323</v>
+        <v>0.3</v>
       </c>
       <c r="G2" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>model_week_365_144</t>
+          <t>model_month_133_72</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.747285842895508</v>
+        <v>2.063173770904541</v>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4696487911301886</v>
+        <v>0.01</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1039155309883323</v>
+        <v>0.3</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H3" t="n">
         <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>0.05</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>model_week_700_72</t>
+          <t>model_month_365_360</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.97217750549316</v>
+        <v>3.133453845977783</v>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01058413796901732</v>
+        <v>0.03</v>
       </c>
       <c r="E4" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2960659121982872</v>
+        <v>0.25</v>
       </c>
       <c r="G4" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H4" t="n">
         <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>0.05</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>model_week_700_144</t>
+          <t>model_month_365_360</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.59808349609375</v>
+        <v>3.346664428710938</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01058413796901732</v>
+        <v>0.03</v>
       </c>
       <c r="E5" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2960659121982872</v>
+        <v>0.25</v>
       </c>
       <c r="G5" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" t="n">
         <v>4</v>
       </c>
       <c r="I5" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -611,115 +611,115 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.07178783416748</v>
+        <v>3.64</v>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05808054277495504</v>
+        <v>0.3118237184625287</v>
       </c>
       <c r="E6" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2997107370422699</v>
+        <v>0.2942142845880926</v>
       </c>
       <c r="G6" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.15</v>
+        <v>0.002283777543696124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>model_month_365_360</t>
+          <t>model_month_365_72</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.236636638641357</v>
+        <v>3.702678680419922</v>
       </c>
       <c r="C7" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05808054277495504</v>
+        <v>0.01</v>
       </c>
       <c r="E7" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2997107370422699</v>
+        <v>0.3</v>
       </c>
       <c r="G7" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>0.15</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>model_month_700_168</t>
+          <t>model_month_365_168</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.57568883895874</v>
+        <v>3.740181922912598</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05808054277495504</v>
+        <v>0.01</v>
       </c>
       <c r="E8" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2997107370422699</v>
+        <v>0.3</v>
       </c>
       <c r="G8" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
-        <v>0.05</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>model_month_700_360</t>
+          <t>model_month_200_72</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.345937252044678</v>
+        <v>3.747611522674561</v>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05808054277495504</v>
+        <v>0.03</v>
       </c>
       <c r="E9" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2997107370422699</v>
+        <v>0.25</v>
       </c>
       <c r="G9" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
@@ -731,26 +731,26 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>model_month_700_504</t>
+          <t>model_month_365_360</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5.529139041900635</v>
+        <v>3.845516681671143</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05808054277495504</v>
+        <v>0.03</v>
       </c>
       <c r="E10" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2997107370422699</v>
+        <v>0.25</v>
       </c>
       <c r="G10" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H10" t="n">
         <v>2</v>
@@ -762,32 +762,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>model_month_700_504</t>
+          <t>model_month_365_168</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.403566360473633</v>
+        <v>4.07178783416748</v>
       </c>
       <c r="C11" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>0.05</v>
+        <v>0.05808054277495504</v>
       </c>
       <c r="E11" t="n">
         <v>32</v>
       </c>
       <c r="F11" t="n">
-        <v>0.25</v>
+        <v>0.2997107370422699</v>
       </c>
       <c r="G11" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="H11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="12">
@@ -797,41 +797,41 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.353591442108154</v>
+        <v>4.297078609466553</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E12" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="G12" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
       </c>
       <c r="I12" t="n">
-        <v>0.001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>model_month_365_168</t>
+          <t>model_month_365_72</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.740181922912598</v>
+        <v>4.353591442108154</v>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
         <v>0.01</v>
@@ -855,45 +855,45 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>model_month_365_72</t>
+          <t>model_month_365_360</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.702678680419922</v>
+        <v>4.596550941467285</v>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E14" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="G14" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>model_month_133_72</t>
+          <t>model_week_133_72</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2.063173770904541</v>
+        <v>5.055328369140625</v>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D15" t="n">
         <v>0.01</v>
@@ -917,187 +917,431 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>model_week_133_72</t>
+          <t>model_month_365_360</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8.389998435974121</v>
+        <v>5.236636638641357</v>
       </c>
       <c r="C16" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01</v>
+        <v>0.05808054277495504</v>
       </c>
       <c r="E16" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3</v>
+        <v>0.2997107370422699</v>
       </c>
       <c r="G16" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I16" t="n">
-        <v>0.001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>model_week_133_72</t>
+          <t>model_month_700_360</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5.055328369140625</v>
+        <v>5.345937252044678</v>
       </c>
       <c r="C17" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01</v>
+        <v>0.05808054277495504</v>
       </c>
       <c r="E17" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3</v>
+        <v>0.2997107370422699</v>
       </c>
       <c r="G17" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>model_week_133_24</t>
+          <t>model_month_700_504</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>13.58229351043701</v>
+        <v>5.529139041900635</v>
       </c>
       <c r="C18" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01</v>
+        <v>0.05808054277495504</v>
       </c>
       <c r="E18" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3</v>
+        <v>0.2997107370422699</v>
       </c>
       <c r="G18" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>model_week_133_24</t>
+          <t>model_month_700_168</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6.060751438140869</v>
+        <v>5.57568883895874</v>
       </c>
       <c r="C19" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01</v>
+        <v>0.05808054277495504</v>
       </c>
       <c r="E19" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3</v>
+        <v>0.2997107370422699</v>
       </c>
       <c r="G19" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>model_month_365_360</t>
+          <t>model_week_133_24</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3.133453845977783</v>
+        <v>6.060751438140869</v>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E20" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F20" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="G20" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H20" t="n">
         <v>4</v>
       </c>
       <c r="I20" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>model_month_365_72</t>
+          <t>model_month_700_504</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4.297078609466553</v>
+        <v>6.403566360473633</v>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D21" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E21" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F21" t="n">
         <v>0.25</v>
       </c>
       <c r="G21" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I21" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>model_week_133_72</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>8.389998435974121</v>
+      </c>
+      <c r="C22" t="n">
+        <v>25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E22" t="n">
+        <v>36</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G22" t="n">
+        <v>22</v>
+      </c>
+      <c r="H22" t="n">
+        <v>4</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>model_week_365_144</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>8.747285842895508</v>
+      </c>
+      <c r="C23" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.4696487911301886</v>
+      </c>
+      <c r="E23" t="n">
+        <v>8</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1039155309883323</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>model_week_365_72</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>10.83476448059082</v>
+      </c>
+      <c r="C24" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.4696487911301886</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1039155309883323</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8</v>
+      </c>
+      <c r="H24" t="n">
+        <v>4</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>model_week_700_144</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>12.59808349609375</v>
+      </c>
+      <c r="C25" t="n">
+        <v>30</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.01058413796901732</v>
+      </c>
+      <c r="E25" t="n">
+        <v>36</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.2960659121982872</v>
+      </c>
+      <c r="G25" t="n">
+        <v>22</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>model_week_700_72</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12.97217750549316</v>
+      </c>
+      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01058413796901732</v>
+      </c>
+      <c r="E26" t="n">
+        <v>36</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.2960659121982872</v>
+      </c>
+      <c r="G26" t="n">
+        <v>22</v>
+      </c>
+      <c r="H26" t="n">
+        <v>4</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>model_week_133_24</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>13.58229351043701</v>
+      </c>
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E27" t="n">
+        <v>36</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>22</v>
+      </c>
+      <c r="H27" t="n">
+        <v>4</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>model_month_365_360</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>30</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E28" t="n">
+        <v>24</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G28" t="n">
+        <v>24</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>model_month_365_360</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>20</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E29" t="n">
+        <v>24</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G29" t="n">
+        <v>24</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>